<commit_message>
Add time and freq
</commit_message>
<xml_diff>
--- a/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
+++ b/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STM32 Projects\Oscilloscope\Project\Oscilloscope\Graphic\assets\texts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Oscilloscope\Project\Oscilloscope\Graphic\assets\texts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B779E4-01F3-4EA1-871C-F5C10D4B0EC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
@@ -275,9 +276,6 @@
     <t>&lt;placeholder&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">1234567890. : - , </t>
-  </si>
-  <si>
     <t>sign</t>
   </si>
   <si>
@@ -356,25 +354,28 @@
     <t>Cursor_us</t>
   </si>
   <si>
-    <t>Cursor_ms</t>
-  </si>
-  <si>
-    <t>Delta :               uS</t>
-  </si>
-  <si>
-    <t>Delta :</t>
-  </si>
-  <si>
     <t>meas_ctrl_menu</t>
   </si>
   <si>
     <t xml:space="preserve">Measure : </t>
+  </si>
+  <si>
+    <t>Time :</t>
+  </si>
+  <si>
+    <t>Cursor_hz</t>
+  </si>
+  <si>
+    <t>Freq :</t>
+  </si>
+  <si>
+    <t>1234567890. : - , umvhzs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,86 +532,86 @@
   </cellXfs>
   <cellStyles count="81">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 2" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
-    <cellStyle name="Normal 14 2" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 16" xfId="9"/>
-    <cellStyle name="Normal 16 2" xfId="10"/>
-    <cellStyle name="Normal 16 3" xfId="11"/>
-    <cellStyle name="Normal 17 2" xfId="12"/>
-    <cellStyle name="Normal 17 3" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 2 4" xfId="17"/>
-    <cellStyle name="Normal 2 5" xfId="18"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 7" xfId="20"/>
-    <cellStyle name="Normal 2 8" xfId="21"/>
-    <cellStyle name="Normal 2 9" xfId="22"/>
-    <cellStyle name="Normal 22" xfId="23"/>
-    <cellStyle name="Normal 22 10" xfId="24"/>
-    <cellStyle name="Normal 22 11" xfId="25"/>
-    <cellStyle name="Normal 22 12" xfId="26"/>
-    <cellStyle name="Normal 22 13" xfId="27"/>
-    <cellStyle name="Normal 22 14" xfId="28"/>
-    <cellStyle name="Normal 22 15" xfId="29"/>
-    <cellStyle name="Normal 22 16" xfId="30"/>
-    <cellStyle name="Normal 22 17" xfId="31"/>
-    <cellStyle name="Normal 22 18" xfId="32"/>
-    <cellStyle name="Normal 22 2" xfId="33"/>
-    <cellStyle name="Normal 22 3" xfId="34"/>
-    <cellStyle name="Normal 22 4" xfId="35"/>
-    <cellStyle name="Normal 22 5" xfId="36"/>
-    <cellStyle name="Normal 22 6" xfId="37"/>
-    <cellStyle name="Normal 22 7" xfId="38"/>
-    <cellStyle name="Normal 22 8" xfId="39"/>
-    <cellStyle name="Normal 22 9" xfId="40"/>
-    <cellStyle name="Normal 23 10" xfId="41"/>
-    <cellStyle name="Normal 23 11" xfId="42"/>
-    <cellStyle name="Normal 23 12" xfId="43"/>
-    <cellStyle name="Normal 23 13" xfId="44"/>
-    <cellStyle name="Normal 23 14" xfId="45"/>
-    <cellStyle name="Normal 23 15" xfId="46"/>
-    <cellStyle name="Normal 23 16" xfId="47"/>
-    <cellStyle name="Normal 23 17" xfId="48"/>
-    <cellStyle name="Normal 23 18" xfId="49"/>
-    <cellStyle name="Normal 23 2" xfId="50"/>
-    <cellStyle name="Normal 23 3" xfId="51"/>
-    <cellStyle name="Normal 23 4" xfId="52"/>
-    <cellStyle name="Normal 23 5" xfId="53"/>
-    <cellStyle name="Normal 23 6" xfId="54"/>
-    <cellStyle name="Normal 23 7" xfId="55"/>
-    <cellStyle name="Normal 23 8" xfId="56"/>
-    <cellStyle name="Normal 23 9" xfId="57"/>
-    <cellStyle name="Normal 25 10" xfId="58"/>
-    <cellStyle name="Normal 25 11" xfId="59"/>
-    <cellStyle name="Normal 25 12" xfId="60"/>
-    <cellStyle name="Normal 25 13" xfId="61"/>
-    <cellStyle name="Normal 25 14" xfId="62"/>
-    <cellStyle name="Normal 25 15" xfId="63"/>
-    <cellStyle name="Normal 25 16" xfId="64"/>
-    <cellStyle name="Normal 25 17" xfId="65"/>
-    <cellStyle name="Normal 25 2" xfId="66"/>
-    <cellStyle name="Normal 25 3" xfId="67"/>
-    <cellStyle name="Normal 25 4" xfId="68"/>
-    <cellStyle name="Normal 25 5" xfId="69"/>
-    <cellStyle name="Normal 25 6" xfId="70"/>
-    <cellStyle name="Normal 25 7" xfId="71"/>
-    <cellStyle name="Normal 25 8" xfId="72"/>
-    <cellStyle name="Normal 25 9" xfId="73"/>
-    <cellStyle name="Normal 3" xfId="74"/>
-    <cellStyle name="Normal 4" xfId="75"/>
-    <cellStyle name="Normal 5" xfId="76"/>
-    <cellStyle name="Normal 6" xfId="77"/>
-    <cellStyle name="Normal 7" xfId="78"/>
-    <cellStyle name="Normal 8" xfId="79"/>
-    <cellStyle name="Normal 9" xfId="80"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 10 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 12" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 13" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 14" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 14 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 15" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 16" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 16 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 16 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 17 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 17 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 3" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 4" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2 5" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 6" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 7" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 2 8" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 2 9" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 22" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 22 10" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 22 11" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 22 12" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 22 13" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 22 14" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 22 15" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 22 16" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 22 17" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 22 18" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 22 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 22 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 22 4" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 22 5" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 22 6" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 22 7" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 22 8" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 22 9" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 23 10" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 23 11" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 23 12" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 23 13" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 23 14" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 23 15" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 23 16" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 23 17" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 23 18" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 23 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 23 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 23 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 23 5" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 23 6" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Normal 23 7" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Normal 23 8" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 23 9" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 25 10" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Normal 25 11" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 25 12" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 25 13" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 25 14" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Normal 25 15" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Normal 25 16" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Normal 25 17" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Normal 25 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Normal 25 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Normal 25 4" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 25 5" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Normal 25 6" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 25 7" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Normal 25 8" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Normal 25 9" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="Normal 3" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 4" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 5" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 6" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 7" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 8" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 9" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -706,7 +707,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="8"/>
       <tableStyleElement type="firstColumn" dxfId="7"/>
       <tableStyleElement type="lastColumn" dxfId="6"/>
@@ -728,33 +729,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:E100" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="B3:E100"/>
-  <sortState ref="B4:E6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="B3:E100" totalsRowShown="0" tableBorderDxfId="1">
+  <autoFilter ref="B3:E100" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:E6">
     <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Typography Name"/>
-    <tableColumn id="2" name="Font"/>
-    <tableColumn id="3" name="Size"/>
-    <tableColumn id="4" name="Bpp"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Typography Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Font"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Size"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Bpp"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I810" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="B3:I810"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table8" displayName="Table8" ref="B3:I810" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="B3:I810" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Text ID"/>
-    <tableColumn id="2" name="Typography Name"/>
-    <tableColumn id="3" name="Alignment"/>
-    <tableColumn id="4" name="GB"/>
-    <tableColumn id="5" name="Add additional language here (1 to 3 capital letters) -"/>
-    <tableColumn id="6" name="Add additional language here (1 to 3 capital letters) - 2"/>
-    <tableColumn id="7" name="Add additional language here (1 to 3 capital letters) - 3"/>
-    <tableColumn id="8" name="Add additional language here (1 to 3 capital letters) - 4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Text ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Typography Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Alignment"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="GB"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Add additional language here (1 to 3 capital letters) -"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Add additional language here (1 to 3 capital letters) - 2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Add additional language here (1 to 3 capital letters) - 3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Add additional language here (1 to 3 capital letters) - 4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,29 +1132,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="3" width="25.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
-    <col min="6" max="10" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" style="1" customWidth="1"/>
+    <col min="6" max="10" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1162,7 @@
       <c r="D2"/>
       <c r="E2"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1242,7 +1243,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value must be a legal Bits per pixel value. (e.g. 1,2,4, or 8)_x000a__x000a_">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value must be a legal Bits per pixel value. (e.g. 1,2,4, or 8)_x000a__x000a_" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Internal Values'!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -1255,24 +1256,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J810"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="1" customWidth="1"/>
-    <col min="7" max="9" width="8.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="8.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -1282,7 +1283,7 @@
       <c r="H1"/>
       <c r="I1"/>
     </row>
-    <row r="2" spans="2:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
@@ -1333,11 +1334,11 @@
         <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1348,10 +1349,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1376,10 +1377,10 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1404,10 +1405,10 @@
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1418,10 +1419,10 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1432,10 +1433,10 @@
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>77</v>
       </c>
@@ -1453,7 +1454,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>78</v>
       </c>
@@ -1471,7 +1472,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>79</v>
       </c>
@@ -1489,7 +1490,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>59</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>61</v>
       </c>
@@ -1535,7 +1536,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>62</v>
       </c>
@@ -1553,7 +1554,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>63</v>
       </c>
@@ -1571,7 +1572,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>64</v>
       </c>
@@ -1589,7 +1590,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>66</v>
       </c>
@@ -1621,7 +1622,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>67</v>
       </c>
@@ -1635,7 +1636,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>31</v>
       </c>
@@ -1649,10 +1650,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
@@ -1694,9 +1695,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>23</v>
@@ -1705,12 +1706,12 @@
         <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>23</v>
@@ -1719,12 +1720,12 @@
         <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
@@ -1733,12 +1734,12 @@
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>23</v>
@@ -1747,16 +1748,16 @@
         <v>11</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>23</v>
@@ -1765,14 +1766,14 @@
         <v>11</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34"/>
@@ -1782,10 +1783,10 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1796,10 +1797,10 @@
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
@@ -1810,10 +1811,10 @@
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>41</v>
       </c>
@@ -1824,10 +1825,10 @@
         <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1841,7 +1842,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1855,9 +1856,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>47</v>
@@ -1866,10 +1867,10 @@
         <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
@@ -1880,10 +1881,10 @@
         <v>11</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1894,10 +1895,10 @@
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1908,10 +1909,10 @@
         <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>52</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>54</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>55</v>
       </c>
@@ -1964,10 +1965,10 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>56</v>
       </c>
@@ -1978,10 +1979,10 @@
         <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>57</v>
       </c>
@@ -1995,9 +1996,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>47</v>
@@ -2006,12 +2007,12 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>47</v>
@@ -2020,16 +2021,16 @@
         <v>11</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>47</v>
@@ -2038,2282 +2039,2282 @@
         <v>11</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D54"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D55"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D62"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D63"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D69"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D70"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D71"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D72"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D73"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D74"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D75"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D76"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D77"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D78"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D79"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D80"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D81"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D82"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D83"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D84"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D85"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D87"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D88"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D89"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D90"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D91"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D92"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D93"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D94"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D95"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D96"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D98"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D99"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D100"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D101"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D102"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D103"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D104"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D105"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D106"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D107"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D108"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D109"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D110"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D111"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D112"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D113"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D114"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D115"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D116"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D117"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D118"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D119"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D120"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D121"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D122"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D123"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D124"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D125"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D126"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D127"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D128"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D161"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D162"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D163"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D164"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D165"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D166"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D167"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D168"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D169"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D170"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D171"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D172"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D173"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D174"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D175"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D176"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D177"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D178"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D179"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D180"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D181"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D182"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D183"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D184"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D185"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D186"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D187"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D188"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D189"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D190"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D191"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D192"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D193"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D194"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D195"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D196"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D197"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D198"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D199"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D200"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D201"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D202"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D203"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D204"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D205"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D206"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D207"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D208"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D209"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D210"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D211"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D212"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D213"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D214"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D215"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D216"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D217"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D218"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D219"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D220"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D221"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D222"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D223"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D224"/>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D225"/>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D226"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D227"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D228"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D229"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D230"/>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D231"/>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D232"/>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D233"/>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D234"/>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D235"/>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D236"/>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D237"/>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D238"/>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D239"/>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D240"/>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D241"/>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D242"/>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D243"/>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D244"/>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D245"/>
     </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D246"/>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D247"/>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D248"/>
     </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D249"/>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D250"/>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D251"/>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D252"/>
     </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D253"/>
     </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D254"/>
     </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D255"/>
     </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D256"/>
     </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D257"/>
     </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D258"/>
     </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D259"/>
     </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D260"/>
     </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D261"/>
     </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D262"/>
     </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D263"/>
     </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D264"/>
     </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D265"/>
     </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D266"/>
     </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D267"/>
     </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D268"/>
     </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D269"/>
     </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D270"/>
     </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D271"/>
     </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D272"/>
     </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D273"/>
     </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D274"/>
     </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D275"/>
     </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D276"/>
     </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D277"/>
     </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D278"/>
     </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D279"/>
     </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D280"/>
     </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D281"/>
     </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D282"/>
     </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D283"/>
     </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D284"/>
     </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D285"/>
     </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D286"/>
     </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D287"/>
     </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D288"/>
     </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D289"/>
     </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D290"/>
     </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D291"/>
     </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D292"/>
     </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D293"/>
     </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D294"/>
     </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D295"/>
     </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D296"/>
     </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D297"/>
     </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D298"/>
     </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D299"/>
     </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D300"/>
     </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D301"/>
     </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D302"/>
     </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D303"/>
     </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D304"/>
     </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D305"/>
     </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D306"/>
     </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D307"/>
     </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D308"/>
     </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D309"/>
     </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D310"/>
     </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D311"/>
     </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D312"/>
     </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D313"/>
     </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D314"/>
     </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D315"/>
     </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D316"/>
     </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D317"/>
     </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D318"/>
     </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D319"/>
     </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D320"/>
     </row>
-    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D321"/>
     </row>
-    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D322"/>
     </row>
-    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D323"/>
     </row>
-    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D324"/>
     </row>
-    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D325"/>
     </row>
-    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D326"/>
     </row>
-    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D327"/>
     </row>
-    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D328"/>
     </row>
-    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D329"/>
     </row>
-    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D330"/>
     </row>
-    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D331"/>
     </row>
-    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D332"/>
     </row>
-    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D333"/>
     </row>
-    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D334"/>
     </row>
-    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D335"/>
     </row>
-    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D336"/>
     </row>
-    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D337"/>
     </row>
-    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D338"/>
     </row>
-    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D339"/>
     </row>
-    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D340"/>
     </row>
-    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D341"/>
     </row>
-    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D342"/>
     </row>
-    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D343"/>
     </row>
-    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D344"/>
     </row>
-    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D345"/>
     </row>
-    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D346"/>
     </row>
-    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D347"/>
     </row>
-    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D348"/>
     </row>
-    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D349"/>
     </row>
-    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D350"/>
     </row>
-    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D351"/>
     </row>
-    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D352"/>
     </row>
-    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D353"/>
     </row>
-    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D354"/>
     </row>
-    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D355"/>
     </row>
-    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D356"/>
     </row>
-    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D357"/>
     </row>
-    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D358"/>
     </row>
-    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D359"/>
     </row>
-    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D360"/>
     </row>
-    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D361"/>
     </row>
-    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D362"/>
     </row>
-    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D363"/>
     </row>
-    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D364"/>
     </row>
-    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D365"/>
     </row>
-    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D366"/>
     </row>
-    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D367"/>
     </row>
-    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D368"/>
     </row>
-    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D369"/>
     </row>
-    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D370"/>
     </row>
-    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D371"/>
     </row>
-    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D372"/>
     </row>
-    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D373"/>
     </row>
-    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D374"/>
     </row>
-    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D375"/>
     </row>
-    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D376"/>
     </row>
-    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D377"/>
     </row>
-    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D378"/>
     </row>
-    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D379"/>
     </row>
-    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D380"/>
     </row>
-    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D381"/>
     </row>
-    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D382"/>
     </row>
-    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D383"/>
     </row>
-    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D384"/>
     </row>
-    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D385"/>
     </row>
-    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D386"/>
     </row>
-    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D387"/>
     </row>
-    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D388"/>
     </row>
-    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D389"/>
     </row>
-    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D390"/>
     </row>
-    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D391"/>
     </row>
-    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D392"/>
     </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D393"/>
     </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D394"/>
     </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D395"/>
     </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D396"/>
     </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D397"/>
     </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D398"/>
     </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D399"/>
     </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D400"/>
     </row>
-    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D401"/>
     </row>
-    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D402"/>
     </row>
-    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D403"/>
     </row>
-    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D404"/>
     </row>
-    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D405"/>
     </row>
-    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D406"/>
     </row>
-    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D407"/>
     </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D408"/>
     </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D409"/>
     </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D410"/>
     </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D411"/>
     </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D412"/>
     </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D413"/>
     </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D414"/>
     </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D415"/>
     </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D416"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D417"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D418"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D419"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D420"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D421"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D422"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D423"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D424"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D425"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D426"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D427"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D428"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D429"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D430"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D431"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D432"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D433"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D434"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D435"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D436"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D437"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D438"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D439"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D440"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D441"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D442"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D443"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D444"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D445"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D446"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D447"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D448"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D449"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D450"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D451"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D452"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D453"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D454"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D455"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D456"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D457"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D458"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D459"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D460"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D461"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D462"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D463"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D464"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D465"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D466"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D467"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D468"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D469"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D470"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D471"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D472"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D473"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D474"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D475"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D476"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D477"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D478"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D479"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D480"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D481"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D482"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D483"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D484"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D485"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D486"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D487"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D488"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D489"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D490"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D491"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D492"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D493"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D494"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D495"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D496"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D497"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D498"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D499"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D500"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D501"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D502"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D503"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D504"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D505"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D506"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D507"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D508"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D509"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D510"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D511"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D512"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D513"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D514"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D515"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D516"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D517"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D518"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D519"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D520"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D521"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D522"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D523"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D524"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D525"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D526"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D527"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D528"/>
     </row>
-    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="529" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D529"/>
     </row>
-    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D530"/>
     </row>
-    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D531"/>
     </row>
-    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D532"/>
     </row>
-    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D533"/>
     </row>
-    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D534"/>
     </row>
-    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D535"/>
     </row>
-    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="536" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D536"/>
     </row>
-    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="537" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D537"/>
     </row>
-    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="538" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D538"/>
     </row>
-    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="539" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D539"/>
     </row>
-    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="540" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D540"/>
     </row>
-    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D541"/>
     </row>
-    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D542"/>
     </row>
-    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D543"/>
     </row>
-    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D544"/>
     </row>
-    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="545" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D545"/>
     </row>
-    <row r="546" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="546" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D546"/>
     </row>
-    <row r="547" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="547" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D547"/>
     </row>
-    <row r="548" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="548" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D548"/>
     </row>
-    <row r="549" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="549" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D549"/>
     </row>
-    <row r="550" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="550" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D550"/>
     </row>
-    <row r="551" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="551" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D551"/>
     </row>
-    <row r="552" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="552" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D552"/>
     </row>
-    <row r="553" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="553" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D553"/>
     </row>
-    <row r="554" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="554" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D554"/>
     </row>
-    <row r="555" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="555" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D555"/>
     </row>
-    <row r="556" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="556" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D556"/>
     </row>
-    <row r="557" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="557" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D557"/>
     </row>
-    <row r="558" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="558" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D558"/>
     </row>
-    <row r="559" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="559" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D559"/>
     </row>
-    <row r="560" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="560" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D560"/>
     </row>
-    <row r="561" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="561" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D561"/>
     </row>
-    <row r="562" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="562" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D562"/>
     </row>
-    <row r="563" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="563" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D563"/>
     </row>
-    <row r="564" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="564" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D564"/>
     </row>
-    <row r="565" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="565" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D565"/>
     </row>
-    <row r="566" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="566" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D566"/>
     </row>
-    <row r="567" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="567" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D567"/>
     </row>
-    <row r="568" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="568" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D568"/>
     </row>
-    <row r="569" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="569" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D569"/>
     </row>
-    <row r="570" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="570" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D570"/>
     </row>
-    <row r="571" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="571" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D571"/>
     </row>
-    <row r="572" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="572" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D572"/>
     </row>
-    <row r="573" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="573" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D573"/>
     </row>
-    <row r="574" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="574" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D574"/>
     </row>
-    <row r="575" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="575" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D575"/>
     </row>
-    <row r="576" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="576" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D576"/>
     </row>
-    <row r="577" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="577" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D577"/>
     </row>
-    <row r="578" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="578" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D578"/>
     </row>
-    <row r="579" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="579" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D579"/>
     </row>
-    <row r="580" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="580" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D580"/>
     </row>
-    <row r="581" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="581" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D581"/>
     </row>
-    <row r="582" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="582" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D582"/>
     </row>
-    <row r="583" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="583" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D583"/>
     </row>
-    <row r="584" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="584" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D584"/>
     </row>
-    <row r="585" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="585" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D585"/>
     </row>
-    <row r="586" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="586" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D586"/>
     </row>
-    <row r="587" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="587" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D587"/>
     </row>
-    <row r="588" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="588" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D588"/>
     </row>
-    <row r="589" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="589" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D589"/>
     </row>
-    <row r="590" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="590" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D590"/>
     </row>
-    <row r="591" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="591" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D591"/>
     </row>
-    <row r="592" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="592" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D592"/>
     </row>
-    <row r="593" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="593" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D593"/>
     </row>
-    <row r="594" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="594" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D594"/>
     </row>
-    <row r="595" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="595" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D595"/>
     </row>
-    <row r="596" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="596" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D596"/>
     </row>
-    <row r="597" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="597" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D597"/>
     </row>
-    <row r="598" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="598" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D598"/>
     </row>
-    <row r="599" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="599" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D599"/>
     </row>
-    <row r="600" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="600" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D600"/>
     </row>
-    <row r="601" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="601" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D601"/>
     </row>
-    <row r="602" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="602" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D602"/>
     </row>
-    <row r="603" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="603" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D603"/>
     </row>
-    <row r="604" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="604" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D604"/>
     </row>
-    <row r="605" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="605" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D605"/>
     </row>
-    <row r="606" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="606" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D606"/>
     </row>
-    <row r="607" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="607" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D607"/>
     </row>
-    <row r="608" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="608" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D608"/>
     </row>
-    <row r="609" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="609" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D609"/>
     </row>
-    <row r="610" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="610" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D610"/>
     </row>
-    <row r="611" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="611" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D611"/>
     </row>
-    <row r="612" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="612" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D612"/>
     </row>
-    <row r="613" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="613" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D613"/>
     </row>
-    <row r="614" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="614" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D614"/>
     </row>
-    <row r="615" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="615" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D615"/>
     </row>
-    <row r="616" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="616" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D616"/>
     </row>
-    <row r="617" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="617" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D617"/>
     </row>
-    <row r="618" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="618" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D618"/>
     </row>
-    <row r="619" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="619" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D619"/>
     </row>
-    <row r="620" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="620" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D620"/>
     </row>
-    <row r="621" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="621" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D621"/>
     </row>
-    <row r="622" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="622" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D622"/>
     </row>
-    <row r="623" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="623" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D623"/>
     </row>
-    <row r="624" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="624" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D624"/>
     </row>
-    <row r="625" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="625" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D625"/>
     </row>
-    <row r="626" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="626" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D626"/>
     </row>
-    <row r="627" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="627" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D627"/>
     </row>
-    <row r="628" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="628" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D628"/>
     </row>
-    <row r="629" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="629" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D629"/>
     </row>
-    <row r="630" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="630" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D630"/>
     </row>
-    <row r="631" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="631" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D631"/>
     </row>
-    <row r="632" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="632" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D632"/>
     </row>
-    <row r="633" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="633" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D633"/>
     </row>
-    <row r="634" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="634" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D634"/>
     </row>
-    <row r="635" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="635" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D635"/>
     </row>
-    <row r="636" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="636" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D636"/>
     </row>
-    <row r="637" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="637" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D637"/>
     </row>
-    <row r="638" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="638" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D638"/>
     </row>
-    <row r="639" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="639" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D639"/>
     </row>
-    <row r="640" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="640" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D640"/>
     </row>
-    <row r="641" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="641" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D641"/>
     </row>
-    <row r="642" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="642" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D642"/>
     </row>
-    <row r="643" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="643" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D643"/>
     </row>
-    <row r="644" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="644" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D644"/>
     </row>
-    <row r="645" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="645" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D645"/>
     </row>
-    <row r="646" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="646" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D646"/>
     </row>
-    <row r="647" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="647" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D647"/>
     </row>
-    <row r="648" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="648" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D648"/>
     </row>
-    <row r="649" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="649" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D649"/>
     </row>
-    <row r="650" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="650" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D650"/>
     </row>
-    <row r="651" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="651" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D651"/>
     </row>
-    <row r="652" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="652" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D652"/>
     </row>
-    <row r="653" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="653" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D653"/>
     </row>
-    <row r="654" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="654" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D654"/>
     </row>
-    <row r="655" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="655" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D655"/>
     </row>
-    <row r="656" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="656" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D656"/>
     </row>
-    <row r="657" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="657" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D657"/>
     </row>
-    <row r="658" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="658" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D658"/>
     </row>
-    <row r="659" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="659" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D659"/>
     </row>
-    <row r="660" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="660" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D660"/>
     </row>
-    <row r="661" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="661" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D661"/>
     </row>
-    <row r="662" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="662" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D662"/>
     </row>
-    <row r="663" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="663" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D663"/>
     </row>
-    <row r="664" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="664" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D664"/>
     </row>
-    <row r="665" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="665" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D665"/>
     </row>
-    <row r="666" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="666" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D666"/>
     </row>
-    <row r="667" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="667" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D667"/>
     </row>
-    <row r="668" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="668" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D668"/>
     </row>
-    <row r="669" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="669" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D669"/>
     </row>
-    <row r="670" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="670" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D670"/>
     </row>
-    <row r="671" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="671" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D671"/>
     </row>
-    <row r="672" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="672" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D672"/>
     </row>
-    <row r="673" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="673" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D673"/>
     </row>
-    <row r="674" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="674" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D674"/>
     </row>
-    <row r="675" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="675" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D675"/>
     </row>
-    <row r="676" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="676" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D676"/>
     </row>
-    <row r="677" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="677" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D677"/>
     </row>
-    <row r="678" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="678" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D678"/>
     </row>
-    <row r="679" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="679" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D679"/>
     </row>
-    <row r="680" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="680" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D680"/>
     </row>
-    <row r="681" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="681" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D681"/>
     </row>
-    <row r="682" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="682" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D682"/>
     </row>
-    <row r="683" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="683" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D683"/>
     </row>
-    <row r="684" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="684" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D684"/>
     </row>
-    <row r="685" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="685" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D685"/>
     </row>
-    <row r="686" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="686" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D686"/>
     </row>
-    <row r="687" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="687" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D687"/>
     </row>
-    <row r="688" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="688" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D688"/>
     </row>
-    <row r="689" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="689" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D689"/>
     </row>
-    <row r="690" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="690" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D690"/>
     </row>
-    <row r="691" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="691" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D691"/>
     </row>
-    <row r="692" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="692" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D692"/>
     </row>
-    <row r="693" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="693" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D693"/>
     </row>
-    <row r="694" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="694" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D694"/>
     </row>
-    <row r="695" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="695" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D695"/>
     </row>
-    <row r="696" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="696" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D696"/>
     </row>
-    <row r="697" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="697" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D697"/>
     </row>
-    <row r="698" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="698" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D698"/>
     </row>
-    <row r="699" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="699" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D699"/>
     </row>
-    <row r="700" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="700" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D700"/>
     </row>
-    <row r="701" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="701" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D701"/>
     </row>
-    <row r="702" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="702" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D702"/>
     </row>
-    <row r="703" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="703" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D703"/>
     </row>
-    <row r="704" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="704" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D704"/>
     </row>
-    <row r="705" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="705" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D705"/>
     </row>
-    <row r="706" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="706" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D706"/>
     </row>
-    <row r="707" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="707" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D707"/>
     </row>
-    <row r="708" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="708" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D708"/>
     </row>
-    <row r="709" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="709" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D709"/>
     </row>
-    <row r="710" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="710" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D710"/>
     </row>
-    <row r="711" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="711" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D711"/>
     </row>
-    <row r="712" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="712" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D712"/>
     </row>
-    <row r="713" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="713" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D713"/>
     </row>
-    <row r="714" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="714" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D714"/>
     </row>
-    <row r="715" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="715" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D715"/>
     </row>
-    <row r="716" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="716" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D716"/>
     </row>
-    <row r="717" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="717" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D717"/>
     </row>
-    <row r="718" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="718" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D718"/>
     </row>
-    <row r="719" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="719" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D719"/>
     </row>
-    <row r="720" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="720" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D720"/>
     </row>
-    <row r="721" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="721" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D721"/>
     </row>
-    <row r="722" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="722" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D722"/>
     </row>
-    <row r="723" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="723" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D723"/>
     </row>
-    <row r="724" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="724" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D724"/>
     </row>
-    <row r="725" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="725" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D725"/>
     </row>
-    <row r="726" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="726" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D726"/>
     </row>
-    <row r="727" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="727" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D727"/>
     </row>
-    <row r="728" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="728" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D728"/>
     </row>
-    <row r="729" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="729" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D729"/>
     </row>
-    <row r="730" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="730" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D730"/>
     </row>
-    <row r="731" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="731" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D731"/>
     </row>
-    <row r="732" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="732" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D732"/>
     </row>
-    <row r="733" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="733" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D733"/>
     </row>
-    <row r="734" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="734" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D734"/>
     </row>
-    <row r="735" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="735" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D735"/>
     </row>
-    <row r="736" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="736" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D736"/>
     </row>
-    <row r="737" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="737" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D737"/>
     </row>
-    <row r="738" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="738" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D738"/>
     </row>
-    <row r="739" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="739" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D739"/>
     </row>
-    <row r="740" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="740" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D740"/>
     </row>
-    <row r="741" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="741" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D741"/>
     </row>
-    <row r="742" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="742" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D742"/>
     </row>
-    <row r="743" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="743" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D743"/>
     </row>
-    <row r="744" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="744" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D744"/>
     </row>
-    <row r="745" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="745" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D745"/>
     </row>
-    <row r="746" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="746" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D746"/>
     </row>
-    <row r="747" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="747" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D747"/>
     </row>
-    <row r="748" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="748" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D748"/>
     </row>
-    <row r="749" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="749" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D749"/>
     </row>
-    <row r="750" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="750" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D750"/>
     </row>
-    <row r="751" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="751" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D751"/>
     </row>
-    <row r="752" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="752" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D752"/>
     </row>
-    <row r="753" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="753" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D753"/>
     </row>
-    <row r="754" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="754" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D754"/>
     </row>
-    <row r="755" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="755" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D755"/>
     </row>
-    <row r="756" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="756" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D756"/>
     </row>
-    <row r="757" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="757" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D757"/>
     </row>
-    <row r="758" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="758" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D758"/>
     </row>
-    <row r="759" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="759" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D759"/>
     </row>
-    <row r="760" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="760" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D760"/>
     </row>
-    <row r="761" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="761" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D761"/>
     </row>
-    <row r="762" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="762" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D762"/>
     </row>
-    <row r="763" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="763" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D763"/>
     </row>
-    <row r="764" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="764" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D764"/>
     </row>
-    <row r="765" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="765" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D765"/>
     </row>
-    <row r="766" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="766" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D766"/>
     </row>
-    <row r="767" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="767" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D767"/>
     </row>
-    <row r="768" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="768" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D768"/>
     </row>
-    <row r="769" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="769" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D769"/>
     </row>
-    <row r="770" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="770" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D770"/>
     </row>
-    <row r="771" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="771" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D771"/>
     </row>
-    <row r="772" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="772" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D772"/>
     </row>
-    <row r="773" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="773" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D773"/>
     </row>
-    <row r="774" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="774" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D774"/>
     </row>
-    <row r="775" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="775" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D775"/>
     </row>
-    <row r="776" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="776" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D776"/>
     </row>
-    <row r="777" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="777" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D777"/>
     </row>
-    <row r="778" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="778" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D778"/>
     </row>
-    <row r="779" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="779" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D779"/>
     </row>
-    <row r="780" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="780" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D780"/>
     </row>
-    <row r="781" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="781" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D781"/>
     </row>
-    <row r="782" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="782" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D782"/>
     </row>
-    <row r="783" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="783" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D783"/>
     </row>
-    <row r="784" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="784" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D784"/>
     </row>
-    <row r="785" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="785" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D785"/>
     </row>
-    <row r="786" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="786" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D786"/>
     </row>
-    <row r="787" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="787" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D787"/>
     </row>
-    <row r="788" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="788" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D788"/>
     </row>
-    <row r="789" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="789" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D789"/>
     </row>
-    <row r="790" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="790" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D790"/>
     </row>
-    <row r="791" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="791" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D791"/>
     </row>
-    <row r="792" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="792" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D792"/>
     </row>
-    <row r="793" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="793" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D793"/>
     </row>
-    <row r="794" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="794" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D794"/>
     </row>
-    <row r="795" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="795" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D795"/>
     </row>
-    <row r="796" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="796" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D796"/>
     </row>
-    <row r="797" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="797" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D797"/>
     </row>
-    <row r="798" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="798" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D798"/>
     </row>
-    <row r="799" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="799" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D799"/>
     </row>
-    <row r="800" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="800" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D800"/>
     </row>
-    <row r="801" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="801" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D801"/>
     </row>
-    <row r="802" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="802" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D802"/>
     </row>
-    <row r="803" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="803" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D803"/>
     </row>
-    <row r="804" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="804" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D804"/>
     </row>
-    <row r="805" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="805" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D805"/>
     </row>
-    <row r="806" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="806" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D806"/>
     </row>
-    <row r="807" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="807" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D807"/>
     </row>
-    <row r="808" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="808" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D808"/>
     </row>
-    <row r="809" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="809" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D809"/>
     </row>
-    <row r="810" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="810" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D810"/>
     </row>
   </sheetData>
@@ -4327,13 +4328,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value entered must be a legal alignment value (e.g. LEFT).">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value entered must be a legal alignment value (e.g. LEFT)." xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Internal Values'!$A$2:$A$48</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D6 D9:D810</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value must be a legal Typography name._x000a__x000a_See Typography sheet for legal names.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value must be a legal Typography name._x000a__x000a_See Typography sheet for legal names." xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Typography!$B$4:$B$100</xm:f>
           </x14:formula1>
@@ -4346,20 +4347,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -4380,7 +4381,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -4396,7 +4397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4404,7 +4405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fix trigger in mv
</commit_message>
<xml_diff>
--- a/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
+++ b/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
@@ -365,10 +365,10 @@
     <t>T-CH 2 :</t>
   </si>
   <si>
-    <t>1234567890. : - , umvHzsV</t>
-  </si>
-  <si>
     <t>Freq  :</t>
+  </si>
+  <si>
+    <t>1234567890. : - , umVHzs</t>
   </si>
 </sst>
 </file>
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J810"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1908,7 +1908,7 @@
         <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>9</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>

</xml_diff>

<commit_message>
add freq and peak to peak detect
</commit_message>
<xml_diff>
--- a/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
+++ b/Project/Oscilloscope/Graphic/assets/texts/texts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="132">
   <si>
     <t>Font</t>
   </si>
@@ -381,6 +381,42 @@
   </si>
   <si>
     <t>1234567890. : - , umVKHzs</t>
+  </si>
+  <si>
+    <t>freq1_label</t>
+  </si>
+  <si>
+    <t>freq2_label</t>
+  </si>
+  <si>
+    <t>pp1_label</t>
+  </si>
+  <si>
+    <t>pp2_label</t>
+  </si>
+  <si>
+    <t>Freq1_value</t>
+  </si>
+  <si>
+    <t>Freq2_value</t>
+  </si>
+  <si>
+    <t>PP1_value</t>
+  </si>
+  <si>
+    <t>PP2_value</t>
+  </si>
+  <si>
+    <t>Pk-Pk(1) :</t>
+  </si>
+  <si>
+    <t>Pk-Pk(2) :</t>
+  </si>
+  <si>
+    <t>Freq(1) :</t>
+  </si>
+  <si>
+    <t>Freq(2) :</t>
   </si>
 </sst>
 </file>
@@ -756,8 +792,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I812" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="B3:I812"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="B3:I809" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="B3:I809"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Text ID"/>
     <tableColumn id="2" name="Typography Name"/>
@@ -1147,7 +1183,7 @@
   <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1191,7 @@
     <col min="1" max="1" width="0.28515625" customWidth="1"/>
     <col min="2" max="3" width="25.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="1" customWidth="1"/>
     <col min="6" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1268,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J812"/>
+  <dimension ref="B1:J809"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,16 +2130,76 @@
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D56"/>
+      <c r="B56" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D57"/>
+      <c r="B57" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D58"/>
+      <c r="B58" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D59"/>
+      <c r="B59" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D60"/>
@@ -2112,60 +2208,120 @@
       <c r="D61"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D62"/>
+      <c r="B62" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D63"/>
+      <c r="B63" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D64"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D66"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D67"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D68"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D69"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D70"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D71"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D72"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D73"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D74"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D75"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D76"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D77"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D78"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D79"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D80"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
@@ -4354,15 +4510,6 @@
     </row>
     <row r="809" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D809"/>
-    </row>
-    <row r="810" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D810"/>
-    </row>
-    <row r="811" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D811"/>
-    </row>
-    <row r="812" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D812"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -4379,13 +4526,13 @@
           <x14:formula1>
             <xm:f>'Internal Values'!$A$2:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D6 D9:D812</xm:sqref>
+          <xm:sqref>D4:D6 D9:D809</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The value must be a legal Typography name._x000a__x000a_See Typography sheet for legal names.">
           <x14:formula1>
             <xm:f>Typography!$B$4:$B$100</xm:f>
           </x14:formula1>
-          <xm:sqref>C4:C6 C9:C812</xm:sqref>
+          <xm:sqref>C4:C6 C9:C809</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>